<commit_message>
Apply Offer filtering to Clean_Offers & rerun all the classifications
</commit_message>
<xml_diff>
--- a/Test_Results.xlsx
+++ b/Test_Results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="247">
   <si>
     <t xml:space="preserve">Descriptions</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t xml:space="preserve">Segment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Label</t>
   </si>
   <si>
     <t xml:space="preserve">ANNOUNCEMENT FOR THE AWARD OF MASTER'S DEGREE 28/ECUM/CFUM/2024 – FerrOx4Power  Research Fellowship - 1 vacancy A call for applications is now open for the attribution of 1 (one) grant of Master's Degree, within the scope of the R&amp;D project Ferroelectric (pseudo)-binary oxides nanofilms for flexible and ultrafast pulsed power electronics, 2022.01740.PTDC, financed by national funds through Foundation for Science and Technology (FCT, IP), through the Operational Program OE, under the following conditions: Scientific Area: Physics, Physics Engineering, Materials Engineering Recipient category: Students enrolled in a Degree courses. Requirement for granting the fellowship: The applicants may apply without prior registration in the course for which the fellowship is open. The requirement to enroll in a degree course will be verified on the date of contracting the fellowship; Only fellowships whose selected applicants present a valid proof of enrollment in a degree course will be contracted, according to the type of the fellowship, issued by the academic services of the Higher Education Institution, indicating, respectively, the academic year or its duration (star and term). Candidates profile: • Mandatory requirements: Graduates in Physics Engineering or Physics. • Requirements under contract: a) enrolment in a master's/Integrated master's degree in the area requested in the public notice (proof of academic qualifications completed by the deadline for applications, including those resulting from academic degree recognition processes); • Preferred factors: experience in the production of thin films by laser ablation or ion-beam sputtering, as well as in their characterization by advanced techniques. Applicants eligibility: Applicants must comply with the eligibility conditions laid down in article 9 of the Research Grants Regulation of the Portuguese Foundation for Science and Technology (2019). Workplan and objectives to be achieved: The work plan involves the preparation by laser ablation or ion-beam sputtering of multilayered thin films based on ferroelectric materials, as well as their structural, chemical, ferroelectric and electrical characterization, among others. Taking advantage of the combination of different materials, the epitaxial deformation at the interfaces between them and their mechanical interaction with selected substrates, the aim is to obtain multilayered thin films with optimized ferroelectric and energy storage properties. Applicable legislation and regulations: Research Fellowship Holder Statutes, approved by Law no. 40/2004 of August 18, in its current version published by Decree-Law no. 123/2019 of august 28; Regulation of Scientific Research Fellowships of the University of Minho (RBIC), published in “Diário da República”, 2nd serie, no. 119, through dispatch no. 6524/2020 of 22-06-2020, ratified by ratification declaration no. 447/2021 of 22-06-2021 and Regulation of Research Studentships and Fellowships (RBI) of the Foundation for Science and Technology, I.P. - in force. Host/Contracting institution and scientific supervision: The workplan will be carried out in the Physics Center of Minho and Porto Universities, in Gualtar, under the scientific guidance of Dr. José Pedro Basto da Silva and Professor Luís Silvino Alves Marques. Fellowship duration: The grant will take place for a period of 3 months, with a provisional starting date on the october of 2024. The fellowship grant is non-renewable. Amount of the research grant: The value stipend (Monthly Maintenance Allowance) is 990,98€ per month, in accordance with the stipends values published by the Foundation for Science and Technology (FCT I.P.) in the country (Annex I – Monthly Stipends Values for the maintenance allowances of the FCT Regulation for Research Studentships and Fellowships) and Annex II of the Regulation of Scientific Research Fellowships of the University of Minho (RBIC), published in “Diário da República”, 2nd serie, no. 119, through dispatch no. 6524/2020 of 22-06-2020, ratified by ratification declaration no. 447/2021 of 22-06-2021, according to the applicable regulation. Payment is made on the 23st of each month, through bank transfer to the Bank Identification Number of the fellow identified in the contractualization process. Other benefits: Reimbursement of Voluntary Social Security (Social Security contributions), corresponding to the 1st level of discounts (for research grants with a total duration 6 months or higher) and personal accident insurance. Exclusivity regime: The grantee will perform the activities under exclusivity, as foreseen in article 5º of the Research Fellow Statutes and applicable regulations. Selection panel: President: José Pedro Basto da Silva, Assistant Researcher, Centre of Physics, School of Sciences of the University of Minho; Effective Member: Mário António Caixeiro Castro Pereira, Assistant Professor, Department of Physics, School of Sciences of the University of Minho; Luís Silvino Alves Marques, Assistant Professor, Department of Physics, School of Sciences of the Minho University; Substitute member: Maria de Jesus de Matos Gomes, Full Professor, Department of Physics, School of Sciences of the Minho University; Veniero Lenzi, Doctoral Researcher, Department of Chemistry from the University of Aveiro. The first effective member will substitute the President of the selection panel in case of impediment, being nominate the first substitute member in the place of the first effective member. Criteria and procedures for applications assessment and selection: The applications assessment will focus on the candidate's Merit, following evaluation criteria, valued on a scale of 1 to 5 values: Applicant Merit - AM (100%): A.1: Academic path (considering the classifications of academic degrees), with a weighting of 50%; A.2: Personal curriculum (considering professional and scientific background), with a weighting of 40%; A.3: Motivation letter, with a weighting of 10%. The final classification of the applicant’s merit with the achieved through the following formula: MC=(A1×0,5) + (A2×0,4) + (A3×0,1) The academic degrees and diplomas documents, or their respective recognition when awarded by foreign higher education institutions are not mandatory in the application phase, being replaced by a declaration of honor of the candidate with the contents of academic results. The documents of academic qualification or respective recognition will be required in the contracting phase and must attest facts that occurred on a date prior to the application. In situations of divergence between the information contained in the declaration and the documentation submitted for contracting the grant, only the information contained in the latter will be consider. If the documents proving the ownership of the academic degree and diploma, or the respective recognition under the terms of Decree-Law No. 66/2018, of August 16, do not correspond to the classifications awarded in the evaluation of the academic path, which can change the candidate's ranking, the fellowship won’t be contracted. Disclosure of results: The provisional results of applications, based in the selection panel minutes, will be send to the applicants by email until 90 working days from the applications deadline. If case of unfavourable results, the candidates have a period of 10 working days to comment, if desired, in a prior hearing to interested parties, pursuant to articles 121 and 122 of the Code of Administrative Procedure (DL no. 4 / 2015 of January 7th). Complaint and appeal procedures: The final results of the evaluation will be published through an ordered list (alphabetically), posted in a visible and public place of the host unit, as well as by email to all applicants, enclosing for that purpose, the minutes of the jury deliberations. The selected candidate must inform its willingness to accept the grant, in writing. In case of rejection, the fellowship will be awarded to the next candidate in the ordered list of applicants. The final decision can be contested within 15 working days, by sending to the President of the jury the corresponding claim. Interested parties may also submit an optional hierarchical appeal, addressed to the Pro-Rector for Research and Projects, Professor Sandra Cristina Almeida Paiva. Application deadline and submission: The call for applications is open for 10 working days from the date of publication of the announcement on the Euraxess portal. Applications must be formalized by sending an application letter with the following documents: curriculum vitae; qualifications certificate or declaration of the applicant; motivation letter; statement proving that meets the conditions for the grant typology, according to the application requirements; other documents important to the evaluation process). Applications must be sent by email to bolsas@ecum.uminho.pt, indicating the reference of the call for applications in Subject: 28/ECUM/CFUM/2024-FerrOx4Power. Applications submitted by other means will not be accepted. Fellowship contractualization: The fellowship will be attributed by signing a fellowship contract between the University of Minho and the fellow, accordingly with the contract minute (annex IV of the Regulation of Research Fellowships of the University of Minho (RBIC), published in Diário da República, 2nd Série, no. 119, through dispatch no. 6524/2020 of 22-06-2020, ratified by ratification declaration no. 447/2021 of 22-06-2021, as indicated in 2.4 of the FCT document: “Rules for Granting and Management of Grants within the scope of R&amp;D projects, including infrastructure projects, the multi-annual financing program for R&amp;D units and other FCT financing instruments (Version 2021)”. The contract may only be concluded after all the documentation required is collected, which must take place within a maximum period of 6 months [including evidences of the academic degrees or diplomas and enrolment in degree courses or non-conferring courses, depending on the type of scholarship]. Once all the documentation has been received, the contracting entity has a period of 60 working days to conclude the scholarship contract. Once received, the fellow must return the contract duly signed within 15 working days. The activities under the fellowship contract can only began after proper authorization by the contracting entity. Term and cancellation of fellowship contracts: Without prejudice to the other causes provided the fellowship regulations (FCT and UMinho) and in the Statute of the Research Fellow, the fellowship ends with the completion of the work plan, as well as with the expiration date for which it was granted or renewed. At the end of the fellowship, the grantee is obliged to present a Final Report of the work carried out, in accordance with the objectives and evaluation criteria defined with the scientific advisor, within 30 days after the end of the scholarship. The final report must be prepared in accordance with Annex I of the Scientific Research Fellowships Regulation of the University of Minho (RBIC), published in Diário da República, 2nd Série, no. 119, through dispatch no. 6524/2020 of 22-06-2020, ratified by ratification declaration no. 447/2021 of 22-06-2021. Research FieldPhysicsEducation LevelMaster Degree or equivalent Skills/QualificationsPlease you can find the information in the Offer Description section Specific RequirementsPlease you can find the information in the Offer Description section BenefitsPlease you can find the information in the Offer Description section Eligibility criteriaPlease you can find the information in the Offer Description section Selection processPlease you can find the information in the Offer Description section Website for additional job detailshttps://www.ecum.uminho.pt/pt/Investigacao/Paginas/Emprego-Cientifico.aspx</t>
@@ -4637,7 +4634,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4671,3509 +4668,3506 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>4</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D7" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="4" t="n">
         <v>0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="C9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="C10" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="C12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="C14" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="C16" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="C18" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="F19" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="C21" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" s="4" t="n">
         <v>0</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="C22" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="C24" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" s="4" t="n">
         <v>4</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="C25" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="C26" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D26" s="4" t="n">
         <v>5</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="C27" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="C28" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="C29" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D29" s="4" t="n">
         <v>4</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="C30" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="C31" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="C32" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="C36" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="C37" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="C40" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D40" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="C41" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D41" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D42" s="4" t="n">
         <v>15</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="C43" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="C44" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="C45" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D45" s="4" t="n">
         <v>0</v>
       </c>
       <c r="E45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="C46" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D46" s="4" t="n">
         <v>0</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="C47" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D47" s="4" t="n">
         <v>4</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="C48" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D49" s="4" t="n">
         <v>8</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="C50" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>109</v>
-      </c>
       <c r="C51" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="C54" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D54" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D56" s="4" t="n">
         <v>0</v>
       </c>
       <c r="E56" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="C58" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>120</v>
-      </c>
       <c r="C59" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="C60" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D60" s="4" t="n">
         <v>10</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="C62" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D62" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E62" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="C63" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D63" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>129</v>
-      </c>
       <c r="C64" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D64" s="4" t="n">
         <v>0</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D65" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F66" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D66" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D67" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C71" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F71" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="456" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C76" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F76" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F76" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D79" s="4" t="n">
         <v>3</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D83" s="4" t="n">
         <v>8</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C84" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>152</v>
       </c>
       <c r="D84" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D85" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D86" s="4" t="n">
         <v>4</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D87" s="4" t="n">
         <v>3</v>
       </c>
       <c r="E87" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F87" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="F87" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D90" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E91" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F91" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D92" s="4" t="n">
         <v>6</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C93" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F93" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D93" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E93" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F93" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E94" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F94" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D95" s="4" t="n">
         <v>10</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D96" s="4" t="n">
         <v>10</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D97" s="4" t="n">
         <v>3</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D101" s="4" t="n">
         <v>7</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D102" s="4" t="n">
         <v>5</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D104" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D107" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E108" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B108" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C108" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D108" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="F108" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B111" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F111" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C111" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D111" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F111" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D112" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D114" s="4" t="n">
         <v>3</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D116" s="4" t="n">
         <v>4</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C117" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D117" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F117" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D117" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="E117" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F117" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D118" s="4" t="n">
         <v>5</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D119" s="4" t="n">
         <v>3</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C120" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F120" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D120" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E120" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F120" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D121" s="4" t="n">
         <v>5</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D122" s="4" t="n">
         <v>5</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D124" s="4" t="n">
         <v>5</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D125" s="4" t="n">
         <v>1</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D126" s="4" t="n">
         <v>10</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B128" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D128" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F128" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C128" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D128" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E128" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F128" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C129" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F129" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D129" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E129" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F129" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D130" s="4" t="n">
         <v>4</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D132" s="4" t="n">
         <v>5</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D135" s="4" t="n">
         <v>5</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D137" s="4" t="n">
         <v>5</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D138" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D139" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D140" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D141" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D142" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F142" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C142" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D142" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E142" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F142" s="3" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C143" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D143" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E143" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F143" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D143" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="E143" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F143" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D144" s="4" t="n">
         <v>5</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D145" s="4" t="n">
         <v>5</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D146" s="4" t="n">
         <v>6</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D147" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E147" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F147" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="F147" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D148" s="4" t="n">
         <v>3</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D150" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D151" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D154" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D155" s="4" t="n">
         <v>3</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D156" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D157" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D158" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F158" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D159" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D160" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F160" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F161" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D162" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F162" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D163" s="4" t="n">
         <v>3</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F163" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D164" s="4" t="n">
         <v>3</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F164" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D165" s="4" t="n">
         <v>5</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D166" s="4" t="n">
         <v>5</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E168" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F168" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D169" s="4" t="n">
         <v>3</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F169" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D170" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D171" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F171" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D172" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F172" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D173" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F173" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B174" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B174" s="3" t="s">
-        <v>245</v>
-      </c>
       <c r="C174" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D174" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F174" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D175" s="4" t="n">
         <v>4</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F175" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D176" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F176" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>